<commit_message>
Updated IHPC processed images and data; Modified time function
</commit_message>
<xml_diff>
--- a/Data/data_IHPC.xlsx
+++ b/Data/data_IHPC.xlsx
@@ -53,6 +53,74 @@
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -345,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -395,22 +463,22 @@
         <v>2</v>
       </c>
       <c r="B2" t="n">
-        <v>36076</v>
+        <v>23489</v>
       </c>
       <c r="C2" t="n">
-        <v>2375</v>
+        <v>1669</v>
       </c>
       <c r="D2" t="n">
-        <v>15.1898947368421</v>
+        <v>14.07369682444578</v>
       </c>
       <c r="E2" t="n">
-        <v>200.2324829101562</v>
+        <v>139.9390258789062</v>
       </c>
       <c r="F2" t="n">
-        <v>313.9984130859375</v>
+        <v>287.9834289550781</v>
       </c>
       <c r="G2" t="n">
-        <v>257.1154479980469</v>
+        <v>213.9612274169922</v>
       </c>
     </row>
     <row r="3">
@@ -418,22 +486,22 @@
         <v>4</v>
       </c>
       <c r="B3" t="n">
-        <v>128485</v>
+        <v>126887</v>
       </c>
       <c r="C3" t="n">
-        <v>4709</v>
+        <v>4473</v>
       </c>
       <c r="D3" t="n">
-        <v>27.28498619664472</v>
+        <v>28.36731500111782</v>
       </c>
       <c r="E3" t="n">
-        <v>173.8271942138672</v>
+        <v>171.6033325195312</v>
       </c>
       <c r="F3" t="n">
-        <v>1186.262451171875</v>
+        <v>1241.945434570312</v>
       </c>
       <c r="G3" t="n">
-        <v>680.0448226928711</v>
+        <v>706.7743835449219</v>
       </c>
     </row>
     <row r="4">
@@ -441,22 +509,22 @@
         <v>5</v>
       </c>
       <c r="B4" t="n">
-        <v>15444</v>
+        <v>14895</v>
       </c>
       <c r="C4" t="n">
-        <v>1119</v>
+        <v>1166</v>
       </c>
       <c r="D4" t="n">
-        <v>13.80160857908847</v>
+        <v>12.77444253859348</v>
       </c>
       <c r="E4" t="n">
-        <v>112.4181442260742</v>
+        <v>113.7035751342773</v>
       </c>
       <c r="F4" t="n">
-        <v>214.6864013671875</v>
+        <v>200.4522705078125</v>
       </c>
       <c r="G4" t="n">
-        <v>163.5522727966309</v>
+        <v>157.0779228210449</v>
       </c>
     </row>
     <row r="5">
@@ -464,22 +532,22 @@
         <v>6</v>
       </c>
       <c r="B5" t="n">
-        <v>57484</v>
+        <v>56773</v>
       </c>
       <c r="C5" t="n">
-        <v>2738</v>
+        <v>2790</v>
       </c>
       <c r="D5" t="n">
-        <v>20.99488677867056</v>
+        <v>20.34874551971326</v>
       </c>
       <c r="E5" t="n">
-        <v>196.9882965087891</v>
+        <v>195.8195953369141</v>
       </c>
       <c r="F5" t="n">
-        <v>448.2550048828125</v>
+        <v>448.7347412109375</v>
       </c>
       <c r="G5" t="n">
-        <v>322.6216506958008</v>
+        <v>322.2771682739258</v>
       </c>
     </row>
     <row r="6">
@@ -487,22 +555,22 @@
         <v>7</v>
       </c>
       <c r="B6" t="n">
-        <v>16104</v>
+        <v>7701</v>
       </c>
       <c r="C6" t="n">
-        <v>1132</v>
+        <v>570</v>
       </c>
       <c r="D6" t="n">
-        <v>14.22614840989399</v>
+        <v>13.51052631578947</v>
       </c>
       <c r="E6" t="n">
-        <v>79.04175567626953</v>
+        <v>85.38103485107422</v>
       </c>
       <c r="F6" t="n">
-        <v>294.3209533691406</v>
+        <v>144.3397369384766</v>
       </c>
       <c r="G6" t="n">
-        <v>186.6813545227051</v>
+        <v>114.8603858947754</v>
       </c>
     </row>
     <row r="7">
@@ -510,22 +578,22 @@
         <v>8</v>
       </c>
       <c r="B7" t="n">
-        <v>7653</v>
+        <v>38520</v>
       </c>
       <c r="C7" t="n">
-        <v>566</v>
+        <v>2210</v>
       </c>
       <c r="D7" t="n">
-        <v>13.52120141342756</v>
+        <v>17.42986425339366</v>
       </c>
       <c r="E7" t="n">
-        <v>84.53908538818359</v>
+        <v>97.80214691162109</v>
       </c>
       <c r="F7" t="n">
-        <v>146.1392974853516</v>
+        <v>682.30078125</v>
       </c>
       <c r="G7" t="n">
-        <v>115.3391914367676</v>
+        <v>390.0514640808105</v>
       </c>
     </row>
     <row r="8">
@@ -533,22 +601,22 @@
         <v>9</v>
       </c>
       <c r="B8" t="n">
-        <v>44333</v>
+        <v>127734</v>
       </c>
       <c r="C8" t="n">
-        <v>2270</v>
+        <v>3329</v>
       </c>
       <c r="D8" t="n">
-        <v>19.52995594713656</v>
+        <v>38.37008110543707</v>
       </c>
       <c r="E8" t="n">
-        <v>110.4040603637695</v>
+        <v>158.8050079345703</v>
       </c>
       <c r="F8" t="n">
-        <v>731.258544921875</v>
+        <v>1267.395141601562</v>
       </c>
       <c r="G8" t="n">
-        <v>420.8313026428223</v>
+        <v>713.1000747680664</v>
       </c>
     </row>
     <row r="9">
@@ -556,22 +624,22 @@
         <v>10</v>
       </c>
       <c r="B9" t="n">
-        <v>126298</v>
+        <v>15948</v>
       </c>
       <c r="C9" t="n">
-        <v>3787</v>
+        <v>1108</v>
       </c>
       <c r="D9" t="n">
-        <v>33.35040929495643</v>
+        <v>14.39350180505415</v>
       </c>
       <c r="E9" t="n">
-        <v>226.1522064208984</v>
+        <v>77.46805572509766</v>
       </c>
       <c r="F9" t="n">
-        <v>934.7611694335938</v>
+        <v>297.8793334960938</v>
       </c>
       <c r="G9" t="n">
-        <v>580.4566879272461</v>
+        <v>187.6736946105957</v>
       </c>
     </row>
     <row r="10">
@@ -579,275 +647,275 @@
         <v>11</v>
       </c>
       <c r="B10" t="n">
-        <v>10921</v>
+        <v>10121</v>
       </c>
       <c r="C10" t="n">
-        <v>695</v>
+        <v>682</v>
       </c>
       <c r="D10" t="n">
-        <v>15.7136690647482</v>
+        <v>14.84017595307918</v>
       </c>
       <c r="E10" t="n">
-        <v>95.61683654785156</v>
+        <v>98.10954284667969</v>
       </c>
       <c r="F10" t="n">
-        <v>171.7776947021484</v>
+        <v>152.2115631103516</v>
       </c>
       <c r="G10" t="n">
-        <v>133.697265625</v>
+        <v>125.1605529785156</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B11" t="n">
-        <v>29279</v>
+        <v>27098</v>
       </c>
       <c r="C11" t="n">
-        <v>1967</v>
+        <v>1885</v>
       </c>
       <c r="D11" t="n">
-        <v>14.88510421962379</v>
+        <v>14.37559681697613</v>
       </c>
       <c r="E11" t="n">
-        <v>108.8709869384766</v>
+        <v>94.80092620849609</v>
       </c>
       <c r="F11" t="n">
-        <v>439.1244201660156</v>
+        <v>455.0233764648438</v>
       </c>
       <c r="G11" t="n">
-        <v>273.9977035522461</v>
+        <v>274.9121513366699</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B12" t="n">
-        <v>22912</v>
+        <v>12965</v>
       </c>
       <c r="C12" t="n">
-        <v>1766</v>
+        <v>1043</v>
       </c>
       <c r="D12" t="n">
-        <v>12.97395243488109</v>
+        <v>12.43048897411314</v>
       </c>
       <c r="E12" t="n">
-        <v>102.2354736328125</v>
+        <v>69.87619018554688</v>
       </c>
       <c r="F12" t="n">
-        <v>363.4148559570312</v>
+        <v>260.612548828125</v>
       </c>
       <c r="G12" t="n">
-        <v>232.8251647949219</v>
+        <v>165.2443695068359</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B13" t="n">
-        <v>87778</v>
+        <v>31391</v>
       </c>
       <c r="C13" t="n">
-        <v>3674</v>
+        <v>2280</v>
       </c>
       <c r="D13" t="n">
-        <v>23.89167120304845</v>
+        <v>13.76798245614035</v>
       </c>
       <c r="E13" t="n">
-        <v>231.286376953125</v>
+        <v>118.4514541625977</v>
       </c>
       <c r="F13" t="n">
-        <v>570.3848266601562</v>
+        <v>413.8274841308594</v>
       </c>
       <c r="G13" t="n">
-        <v>400.8356018066406</v>
+        <v>266.1394691467285</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B14" t="n">
-        <v>44770</v>
+        <v>88898</v>
       </c>
       <c r="C14" t="n">
-        <v>3110</v>
+        <v>3981</v>
       </c>
       <c r="D14" t="n">
-        <v>14.39549839228296</v>
+        <v>22.33057020849033</v>
       </c>
       <c r="E14" t="n">
-        <v>118.357421875</v>
+        <v>275.7662353515625</v>
       </c>
       <c r="F14" t="n">
-        <v>689.370849609375</v>
+        <v>557.4521484375</v>
       </c>
       <c r="G14" t="n">
-        <v>403.8641357421875</v>
+        <v>416.6091918945312</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B15" t="n">
-        <v>40171</v>
+        <v>9415</v>
       </c>
       <c r="C15" t="n">
-        <v>3133</v>
+        <v>843</v>
       </c>
       <c r="D15" t="n">
-        <v>12.82189594637727</v>
+        <v>11.16844602609727</v>
       </c>
       <c r="E15" t="n">
-        <v>207.0707244873047</v>
+        <v>87.38130187988281</v>
       </c>
       <c r="F15" t="n">
-        <v>386.1992492675781</v>
+        <v>151.11572265625</v>
       </c>
       <c r="G15" t="n">
-        <v>296.6349868774414</v>
+        <v>119.2485122680664</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B16" t="n">
-        <v>10785</v>
+        <v>36582</v>
       </c>
       <c r="C16" t="n">
-        <v>905</v>
+        <v>2823</v>
       </c>
       <c r="D16" t="n">
-        <v>11.9171270718232</v>
+        <v>12.95855472901169</v>
       </c>
       <c r="E16" t="n">
-        <v>65.97031402587891</v>
+        <v>186.0671997070312</v>
       </c>
       <c r="F16" t="n">
-        <v>215.3141937255859</v>
+        <v>385.9921569824219</v>
       </c>
       <c r="G16" t="n">
-        <v>140.6422538757324</v>
+        <v>286.0296783447266</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B17" t="n">
-        <v>47035</v>
+        <v>25451</v>
       </c>
       <c r="C17" t="n">
-        <v>2857</v>
+        <v>1591</v>
       </c>
       <c r="D17" t="n">
-        <v>16.46307315365768</v>
+        <v>15.99685732243872</v>
       </c>
       <c r="E17" t="n">
-        <v>183.1996917724609</v>
+        <v>116.950065612793</v>
       </c>
       <c r="F17" t="n">
-        <v>433.3032531738281</v>
+        <v>321.0515441894531</v>
       </c>
       <c r="G17" t="n">
-        <v>308.2514724731445</v>
+        <v>219.000804901123</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B18" t="n">
-        <v>95299</v>
+        <v>30999</v>
       </c>
       <c r="C18" t="n">
-        <v>5054</v>
+        <v>2083</v>
       </c>
       <c r="D18" t="n">
-        <v>18.85615354174911</v>
+        <v>14.88190110417667</v>
       </c>
       <c r="E18" t="n">
-        <v>267.8778381347656</v>
+        <v>103.4430923461914</v>
       </c>
       <c r="F18" t="n">
-        <v>687.49462890625</v>
+        <v>492.1207275390625</v>
       </c>
       <c r="G18" t="n">
-        <v>477.6862335205078</v>
+        <v>297.781909942627</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B19" t="n">
-        <v>46040</v>
+        <v>7917</v>
       </c>
       <c r="C19" t="n">
-        <v>2333</v>
+        <v>678</v>
       </c>
       <c r="D19" t="n">
-        <v>19.73424774967853</v>
+        <v>11.67699115044248</v>
       </c>
       <c r="E19" t="n">
-        <v>85.61701965332031</v>
+        <v>64.07973480224609</v>
       </c>
       <c r="F19" t="n">
-        <v>781.2774658203125</v>
+        <v>163.9772338867188</v>
       </c>
       <c r="G19" t="n">
-        <v>433.4472427368164</v>
+        <v>114.0284843444824</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B20" t="n">
-        <v>20293</v>
+        <v>93394</v>
       </c>
       <c r="C20" t="n">
-        <v>1400</v>
+        <v>5085</v>
       </c>
       <c r="D20" t="n">
-        <v>14.495</v>
+        <v>18.36656833824975</v>
       </c>
       <c r="E20" t="n">
-        <v>68.54212951660156</v>
+        <v>281.6588745117188</v>
       </c>
       <c r="F20" t="n">
-        <v>437.7068176269531</v>
+        <v>683.6231079101562</v>
       </c>
       <c r="G20" t="n">
-        <v>253.1244735717773</v>
+        <v>482.6409912109375</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B21" t="n">
-        <v>20998</v>
+        <v>46514</v>
       </c>
       <c r="C21" t="n">
-        <v>1345</v>
+        <v>2524</v>
       </c>
       <c r="D21" t="n">
-        <v>15.61189591078067</v>
+        <v>18.42868462757528</v>
       </c>
       <c r="E21" t="n">
-        <v>72.14044952392578</v>
+        <v>86.75746154785156</v>
       </c>
       <c r="F21" t="n">
-        <v>395.9342651367188</v>
+        <v>835.8033447265625</v>
       </c>
       <c r="G21" t="n">
-        <v>234.0373573303223</v>
+        <v>461.280403137207</v>
       </c>
     </row>
     <row r="22">
@@ -855,137 +923,206 @@
         <v>36</v>
       </c>
       <c r="B22" t="n">
-        <v>27130</v>
+        <v>14721</v>
       </c>
       <c r="C22" t="n">
-        <v>1221</v>
+        <v>1300</v>
       </c>
       <c r="D22" t="n">
-        <v>22.21949221949222</v>
+        <v>11.32384615384615</v>
       </c>
       <c r="E22" t="n">
-        <v>99.03777313232422</v>
+        <v>114.6783676147461</v>
       </c>
       <c r="F22" t="n">
-        <v>406.9027709960938</v>
+        <v>222.7246704101562</v>
       </c>
       <c r="G22" t="n">
-        <v>252.970272064209</v>
+        <v>168.7015190124512</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B23" t="n">
-        <v>22370</v>
+        <v>20253</v>
       </c>
       <c r="C23" t="n">
-        <v>1780</v>
+        <v>1421</v>
       </c>
       <c r="D23" t="n">
-        <v>12.56741573033708</v>
+        <v>14.25263898662913</v>
       </c>
       <c r="E23" t="n">
-        <v>95.57505798339844</v>
+        <v>68.26117706298828</v>
       </c>
       <c r="F23" t="n">
-        <v>356.7332153320312</v>
+        <v>441.7120056152344</v>
       </c>
       <c r="G23" t="n">
-        <v>226.1541366577148</v>
+        <v>254.9865913391113</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B24" t="n">
-        <v>23971</v>
+        <v>20163</v>
       </c>
       <c r="C24" t="n">
-        <v>1080</v>
+        <v>1285</v>
       </c>
       <c r="D24" t="n">
-        <v>22.19537037037037</v>
+        <v>15.69105058365759</v>
       </c>
       <c r="E24" t="n">
-        <v>109.6232757568359</v>
+        <v>72.34642791748047</v>
       </c>
       <c r="F24" t="n">
-        <v>311.1911315917969</v>
+        <v>372.8340454101562</v>
       </c>
       <c r="G24" t="n">
-        <v>210.4072036743164</v>
+        <v>222.5902366638184</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="B25" t="n">
-        <v>16236</v>
+        <v>7811</v>
       </c>
       <c r="C25" t="n">
-        <v>718</v>
+        <v>728</v>
       </c>
       <c r="D25" t="n">
-        <v>22.61281337047354</v>
+        <v>10.7293956043956</v>
       </c>
       <c r="E25" t="n">
-        <v>111.3753662109375</v>
+        <v>79.05519104003906</v>
       </c>
       <c r="F25" t="n">
-        <v>218.4467620849609</v>
+        <v>142.3079528808594</v>
       </c>
       <c r="G25" t="n">
-        <v>164.9110641479492</v>
+        <v>110.6815719604492</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B26" t="n">
-        <v>7814</v>
+        <v>27038</v>
       </c>
       <c r="C26" t="n">
-        <v>400</v>
+        <v>1295</v>
       </c>
       <c r="D26" t="n">
-        <v>19.535</v>
+        <v>20.87876447876448</v>
       </c>
       <c r="E26" t="n">
-        <v>50.88002395629883</v>
+        <v>96.73746490478516</v>
       </c>
       <c r="F26" t="n">
-        <v>203.5180206298828</v>
+        <v>432.50927734375</v>
       </c>
       <c r="G26" t="n">
-        <v>127.1990222930908</v>
+        <v>264.6233711242676</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B27" t="n">
-        <v>8233</v>
+        <v>26604</v>
       </c>
       <c r="C27" t="n">
-        <v>580</v>
+        <v>2174</v>
       </c>
       <c r="D27" t="n">
-        <v>14.1948275862069</v>
+        <v>12.23735050597976</v>
       </c>
       <c r="E27" t="n">
-        <v>58.63681793212891</v>
+        <v>155.4207000732422</v>
       </c>
       <c r="F27" t="n">
-        <v>211.5411987304688</v>
+        <v>335.85791015625</v>
       </c>
       <c r="G27" t="n">
-        <v>135.0890083312988</v>
+        <v>245.6393051147461</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>47</v>
+      </c>
+      <c r="B28" t="n">
+        <v>23789</v>
+      </c>
+      <c r="C28" t="n">
+        <v>1136</v>
+      </c>
+      <c r="D28" t="n">
+        <v>20.94102112676056</v>
+      </c>
+      <c r="E28" t="n">
+        <v>107.7107086181641</v>
+      </c>
+      <c r="F28" t="n">
+        <v>314.014892578125</v>
+      </c>
+      <c r="G28" t="n">
+        <v>210.8628005981445</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>54</v>
+      </c>
+      <c r="B29" t="n">
+        <v>15958</v>
+      </c>
+      <c r="C29" t="n">
+        <v>703</v>
+      </c>
+      <c r="D29" t="n">
+        <v>22.69985775248933</v>
+      </c>
+      <c r="E29" t="n">
+        <v>111.2905654907227</v>
+      </c>
+      <c r="F29" t="n">
+        <v>213.9639739990234</v>
+      </c>
+      <c r="G29" t="n">
+        <v>162.627269744873</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>55</v>
+      </c>
+      <c r="B30" t="n">
+        <v>8198</v>
+      </c>
+      <c r="C30" t="n">
+        <v>579</v>
+      </c>
+      <c r="D30" t="n">
+        <v>14.15889464594128</v>
+      </c>
+      <c r="E30" t="n">
+        <v>58.04082107543945</v>
+      </c>
+      <c r="F30" t="n">
+        <v>208.79833984375</v>
+      </c>
+      <c r="G30" t="n">
+        <v>133.4195804595947</v>
       </c>
     </row>
   </sheetData>

</xml_diff>